<commit_message>
se crearon mas nan
</commit_message>
<xml_diff>
--- a/DATOS200.xlsx
+++ b/DATOS200.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crrb\Documents\GitHub\DIPLOM_BIGDATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B4E7F3-EB39-4852-8D62-999501056AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52976889-CBDE-4CD2-89F1-BBEB2F3B6342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="12">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -413,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="D196" sqref="D196"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,9 +507,6 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
       <c r="B7">
         <v>89</v>
       </c>
@@ -725,9 +722,6 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
       <c r="B24">
         <v>77</v>
       </c>
@@ -1367,9 +1361,6 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>5</v>
-      </c>
       <c r="B71">
         <v>26</v>
       </c>
@@ -3131,9 +3122,6 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>11</v>
-      </c>
       <c r="B200">
         <v>76</v>
       </c>
@@ -3148,15 +3136,10 @@
       <c r="A201" t="s">
         <v>4</v>
       </c>
-      <c r="B201">
-        <v>83</v>
-      </c>
       <c r="C201">
         <v>82.98</v>
       </c>
-      <c r="D201" s="1">
-        <v>44774.796759259261</v>
-      </c>
+      <c r="D201" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>